<commit_message>
feat: Enhanced Ingestion UI and robust Trend Calculation Logic (Sold assets nullification, Historical overwrite fix)
</commit_message>
<xml_diff>
--- a/0. Dati Iniziali/PortfolioMP_Prezzi_LATEST.xlsx
+++ b/0. Dati Iniziali/PortfolioMP_Prezzi_LATEST.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\PerixMonitor\0. Dati Iniziali\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBBDF6A2-98F8-4BAC-8ABE-216F328523CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BED67AEA-B45E-4A13-A561-DFE2BF8739E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{461EA0C3-CC98-4DCD-BC5C-C997A9959903}"/>
+    <workbookView xWindow="-110" yWindow="490" windowWidth="38620" windowHeight="21220" xr2:uid="{461EA0C3-CC98-4DCD-BC5C-C997A9959903}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -329,7 +329,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -366,6 +366,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -500,7 +512,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -577,6 +589,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1404,11 +1423,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{840B4B52-5CB9-41B5-89C1-B1D0A0795C06}">
-  <dimension ref="A1:M20"/>
+  <dimension ref="A1:O20"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5:XFD5"/>
+      <selection pane="bottomLeft" activeCell="I5" sqref="I5:I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1422,12 +1441,12 @@
     <col min="7" max="7" width="16.54296875" customWidth="1"/>
     <col min="8" max="8" width="22.26953125" customWidth="1"/>
     <col min="9" max="9" width="21.90625" customWidth="1"/>
-    <col min="11" max="11" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.6328125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17.90625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="19.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -1457,13 +1476,13 @@
       </c>
       <c r="K1" s="22">
         <f>SUM(K2:K19)</f>
-        <v>486324.66348221997</v>
+        <v>489607.11841121991</v>
       </c>
       <c r="L1" s="21" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="23" t="s">
         <v>27</v>
       </c>
@@ -1480,7 +1499,7 @@
         <v>100</v>
       </c>
       <c r="F2" s="19">
-        <v>46053</v>
+        <v>46055</v>
       </c>
       <c r="G2" s="18"/>
       <c r="H2" s="20"/>
@@ -1492,7 +1511,7 @@
         <v>10017.950499999999</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" s="23" t="s">
         <v>29</v>
       </c>
@@ -1509,19 +1528,19 @@
         <v>94.621300000000005</v>
       </c>
       <c r="F3" s="19">
-        <v>46053</v>
+        <v>46055</v>
       </c>
       <c r="G3" s="18"/>
       <c r="H3" s="20"/>
       <c r="I3" s="33">
-        <v>94.73</v>
+        <v>95.4</v>
       </c>
       <c r="K3" s="35">
         <f t="shared" ref="K3:K19" si="0">+C3*I3</f>
-        <v>14683.150000000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+        <v>14787</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" s="23" t="s">
         <v>13</v>
       </c>
@@ -1538,19 +1557,19 @@
         <v>90.380700000000004</v>
       </c>
       <c r="F4" s="19">
-        <v>46053</v>
+        <v>46055</v>
       </c>
       <c r="G4" s="18"/>
       <c r="H4" s="20"/>
       <c r="I4" s="33">
-        <v>98.91</v>
+        <v>98.92</v>
       </c>
       <c r="K4" s="35">
         <f t="shared" si="0"/>
-        <v>24727.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+        <v>24730</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" s="23" t="s">
         <v>11</v>
       </c>
@@ -1567,22 +1586,27 @@
         <v>31.14</v>
       </c>
       <c r="F5" s="19">
-        <v>46053</v>
+        <v>46055</v>
       </c>
       <c r="G5" s="18"/>
       <c r="H5" s="20"/>
-      <c r="I5" s="33">
-        <v>33.770000000000003</v>
+      <c r="I5" s="37">
+        <v>38.1601</v>
       </c>
       <c r="K5" s="35">
         <f t="shared" si="0"/>
-        <v>26553.013300000002</v>
-      </c>
-      <c r="M5" s="35">
-        <v>22472.17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+        <v>30004.905028999998</v>
+      </c>
+      <c r="M5" s="35"/>
+      <c r="N5" s="36">
+        <v>0.13</v>
+      </c>
+      <c r="O5">
+        <f>+I5*(1+N5)</f>
+        <v>43.120912999999994</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" s="23" t="s">
         <v>16</v>
       </c>
@@ -1599,23 +1623,27 @@
         <v>8.8187999999999995</v>
       </c>
       <c r="F6" s="19">
-        <v>46053</v>
+        <v>46055</v>
       </c>
       <c r="G6" s="18"/>
       <c r="H6" s="20"/>
-      <c r="I6" s="33">
-        <v>9.07</v>
+      <c r="I6" s="37">
+        <v>9.307500000000001</v>
       </c>
       <c r="K6" s="35">
         <f t="shared" si="0"/>
-        <v>5169.9000000000005</v>
-      </c>
-      <c r="M6" s="35">
-        <f>+K5-M5</f>
-        <v>4080.8433000000041</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+        <v>5305.2750000000005</v>
+      </c>
+      <c r="M6" s="35"/>
+      <c r="N6" s="36">
+        <v>0.02</v>
+      </c>
+      <c r="O6">
+        <f>+I6*(1+N6)</f>
+        <v>9.4936500000000006</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" s="23" t="s">
         <v>30</v>
       </c>
@@ -1632,23 +1660,27 @@
         <v>42.381100000000004</v>
       </c>
       <c r="F7" s="19">
-        <v>46053</v>
+        <v>46055</v>
       </c>
       <c r="G7" s="18"/>
       <c r="H7" s="20"/>
-      <c r="I7" s="33">
-        <v>40.47</v>
+      <c r="I7" s="38">
+        <v>37.2286</v>
       </c>
       <c r="K7" s="35">
         <f t="shared" si="0"/>
-        <v>9591.39</v>
-      </c>
-      <c r="M7" s="35">
-        <f>+M6+482243.82</f>
-        <v>486324.66330000001</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+        <v>8823.1782000000003</v>
+      </c>
+      <c r="M7" s="35"/>
+      <c r="N7" s="36">
+        <v>-0.03</v>
+      </c>
+      <c r="O7">
+        <f>+I7*(1+N7)</f>
+        <v>36.111742</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" s="23" t="s">
         <v>14</v>
       </c>
@@ -1665,7 +1697,7 @@
         <v>79.260800000000003</v>
       </c>
       <c r="F8" s="19">
-        <v>46053</v>
+        <v>46055</v>
       </c>
       <c r="G8" s="18"/>
       <c r="H8" s="20"/>
@@ -1677,7 +1709,7 @@
         <v>124212.53416</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" s="23" t="s">
         <v>15</v>
       </c>
@@ -1694,7 +1726,7 @@
         <v>188.8296</v>
       </c>
       <c r="F9" s="19">
-        <v>46053</v>
+        <v>46055</v>
       </c>
       <c r="G9" s="18"/>
       <c r="H9" s="20"/>
@@ -1707,7 +1739,7 @@
       </c>
       <c r="M9" s="35"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" s="23" t="s">
         <v>17</v>
       </c>
@@ -1724,19 +1756,19 @@
         <v>108.09699999999999</v>
       </c>
       <c r="F10" s="19">
-        <v>46053</v>
+        <v>46055</v>
       </c>
       <c r="G10" s="18"/>
       <c r="H10" s="20"/>
       <c r="I10" s="33">
-        <v>112.19</v>
+        <v>112.51</v>
       </c>
       <c r="K10" s="35">
         <f t="shared" si="0"/>
-        <v>5272.93</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+        <v>5287.97</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" s="23" t="s">
         <v>18</v>
       </c>
@@ -1753,7 +1785,7 @@
         <v>16.910799999999998</v>
       </c>
       <c r="F11" s="19">
-        <v>46053</v>
+        <v>46055</v>
       </c>
       <c r="G11" s="18"/>
       <c r="H11" s="20"/>
@@ -1765,7 +1797,7 @@
         <v>20204.585586899997</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" s="23" t="s">
         <v>20</v>
       </c>
@@ -1782,7 +1814,7 @@
         <v>183.25</v>
       </c>
       <c r="F12" s="19">
-        <v>46053</v>
+        <v>46055</v>
       </c>
       <c r="G12" s="18"/>
       <c r="H12" s="20"/>
@@ -1794,7 +1826,7 @@
         <v>18696.255658079997</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13" s="23" t="s">
         <v>21</v>
       </c>
@@ -1811,7 +1843,7 @@
         <v>86.142099999999999</v>
       </c>
       <c r="F13" s="19">
-        <v>46053</v>
+        <v>46055</v>
       </c>
       <c r="G13" s="18"/>
       <c r="H13" s="20"/>
@@ -1823,7 +1855,7 @@
         <v>28142.171354440005</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" s="23" t="s">
         <v>22</v>
       </c>
@@ -1840,7 +1872,7 @@
         <v>24.51</v>
       </c>
       <c r="F14" s="19">
-        <v>46053</v>
+        <v>46055</v>
       </c>
       <c r="G14" s="18"/>
       <c r="H14" s="20"/>
@@ -1852,7 +1884,7 @@
         <v>15897.265753600001</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15" s="23" t="s">
         <v>23</v>
       </c>
@@ -1869,7 +1901,7 @@
         <v>188.49709999999999</v>
       </c>
       <c r="F15" s="19">
-        <v>46053</v>
+        <v>46055</v>
       </c>
       <c r="G15" s="18"/>
       <c r="H15" s="20"/>
@@ -1881,7 +1913,7 @@
         <v>24883.093867200001</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16" s="23" t="s">
         <v>25</v>
       </c>
@@ -1898,7 +1930,7 @@
         <v>17.7333</v>
       </c>
       <c r="F16" s="19">
-        <v>46053</v>
+        <v>46055</v>
       </c>
       <c r="G16" s="18"/>
       <c r="H16" s="20"/>
@@ -1927,16 +1959,16 @@
         <v>1009.4647</v>
       </c>
       <c r="F17" s="19">
-        <v>46053</v>
+        <v>46055</v>
       </c>
       <c r="G17" s="18"/>
       <c r="H17" s="20"/>
       <c r="I17" s="33">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="K17" s="35">
         <f t="shared" si="0"/>
-        <v>15090</v>
+        <v>15075</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
@@ -1956,16 +1988,16 @@
         <v>97.022000000000006</v>
       </c>
       <c r="F18" s="19">
-        <v>46053</v>
+        <v>46055</v>
       </c>
       <c r="G18" s="18"/>
       <c r="H18" s="20"/>
       <c r="I18" s="33">
-        <v>97.85</v>
+        <v>99</v>
       </c>
       <c r="K18" s="35">
         <f t="shared" si="0"/>
-        <v>20059.25</v>
+        <v>20295</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1985,16 +2017,16 @@
         <v>93.194999999999993</v>
       </c>
       <c r="F19" s="19">
-        <v>46053</v>
+        <v>46055</v>
       </c>
       <c r="G19" s="18"/>
       <c r="H19" s="20"/>
       <c r="I19" s="34">
-        <v>96.8</v>
+        <v>98.21</v>
       </c>
       <c r="K19" s="35">
         <f t="shared" si="0"/>
-        <v>8324.7999999999993</v>
+        <v>8446.06</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
@@ -2021,7 +2053,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="1" stopIfTrue="1" operator="containsText" id="{3AE5DE67-15A2-4F9B-AC82-395C205EEE6F}">
+          <x14:cfRule type="containsText" priority="1" stopIfTrue="1" operator="containsText" id="{983253CC-52ED-4C0F-8FE7-E0961D3C14A9}">
             <xm:f>NOT(ISERROR(SEARCH("-",D2)))</xm:f>
             <xm:f>"-"</xm:f>
             <x14:dxf>

</xml_diff>

<commit_message>
feat: Separazione Cedole/Dividendi e Spese con colonna type
- Aggiunta colonna 'type' (DIVIDEND/EXPENSE) alla tabella dividends
- Vincolo di unicità aggiornato a (portfolio_id, asset_id, date, type)
- Backfill automatico: importi negativi classificati come EXPENSE
- Aggregazione nel parsing separata per tipo (ISIN + data + tipo)
- API /api/ingest: lookup DB completo con totali per asset (tutte le date)
- API /api/sync: salvataggio con campo type e nuovo on_conflict
- ReconciliationModal: layout adattivo con sezioni separate per cedole e spese
  - Colonne: In Archivio (totale DB) | Nuovi Incassi/Costi | Dopo Importazione
  - Wording dinamico in base al contenuto del file
- UploadForm: gestione stato dividendDelta con tipo
- Migration DB applicata in locale e produzione
</commit_message>
<xml_diff>
--- a/0. Dati Iniziali/PortfolioMP_Prezzi_LATEST.xlsx
+++ b/0. Dati Iniziali/PortfolioMP_Prezzi_LATEST.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\PerixMonitor\0. Dati Iniziali\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B1CA8DB-61D8-461D-B590-970D48000E59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFEF192B-38B2-4C60-AEA1-57CF9216BE06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="600" windowWidth="19200" windowHeight="21000" xr2:uid="{461EA0C3-CC98-4DCD-BC5C-C997A9959903}"/>
+    <workbookView xWindow="-110" yWindow="490" windowWidth="38620" windowHeight="21220" xr2:uid="{461EA0C3-CC98-4DCD-BC5C-C997A9959903}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
     <author>Mauro Periccioli</author>
   </authors>
   <commentList>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{7783A90E-7FBD-4BD0-909A-B9C6CF3DE99A}">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{3EFADE7E-CD35-4438-A69D-9133C9A23942}">
       <text>
         <r>
           <rPr>
@@ -72,7 +72,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I2" authorId="0" shapeId="0" xr:uid="{F3EA6C4C-02C9-4399-B379-A03F8AF902E3}">
+    <comment ref="G2" authorId="0" shapeId="0" xr:uid="{F3EA6C4C-02C9-4399-B379-A03F8AF902E3}">
       <text>
         <r>
           <rPr>
@@ -101,7 +101,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="54">
   <si>
     <t>Descrizione Titolo</t>
   </si>
@@ -118,18 +118,9 @@
     <t>Prezzo Carico (EUR)</t>
   </si>
   <si>
-    <t>Data (acquisto/vendita)</t>
-  </si>
-  <si>
-    <t>Operazione</t>
-  </si>
-  <si>
     <t>Prezzo Corrente (EUR)</t>
   </si>
   <si>
-    <t>Prezzo Operazione (EUR)</t>
-  </si>
-  <si>
     <t>LU0345361124</t>
   </si>
   <si>
@@ -266,6 +257,12 @@
   </si>
   <si>
     <t>Controvalore Totale:</t>
+  </si>
+  <si>
+    <t>Descrizione Asset</t>
+  </si>
+  <si>
+    <t>Data</t>
   </si>
 </sst>
 </file>
@@ -274,10 +271,10 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
     <numFmt numFmtId="8" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-    <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
     <numFmt numFmtId="165" formatCode="#,##0.00;;\-"/>
     <numFmt numFmtId="166" formatCode="0.0000"/>
     <numFmt numFmtId="167" formatCode="#,##0.0000\ &quot;€&quot;;[Red]\-#,##0.0000\ &quot;€&quot;"/>
+    <numFmt numFmtId="168" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;;\-"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -326,18 +323,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor theme="9"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -360,6 +351,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -460,15 +463,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -476,36 +472,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="8" fontId="4" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="4" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -517,9 +509,16 @@
     <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -619,7 +618,7 @@
             <v>100</v>
           </cell>
           <cell r="J7">
-            <v>46056.366570081016</v>
+            <v>46059.648170324072</v>
           </cell>
           <cell r="L7">
             <v>100.77</v>
@@ -642,10 +641,10 @@
             <v>94.621300000000005</v>
           </cell>
           <cell r="J8">
-            <v>46056.366570081016</v>
+            <v>46059.648170324072</v>
           </cell>
           <cell r="L8">
-            <v>95.99</v>
+            <v>87.06</v>
           </cell>
         </row>
         <row r="9">
@@ -665,10 +664,10 @@
             <v>90.380700000000004</v>
           </cell>
           <cell r="J9">
-            <v>46056.366570081016</v>
+            <v>46059.648170324072</v>
           </cell>
           <cell r="L9">
-            <v>98.96</v>
+            <v>98.94</v>
           </cell>
         </row>
         <row r="10">
@@ -688,10 +687,10 @@
             <v>31.14</v>
           </cell>
           <cell r="J10">
-            <v>46056.366570081016</v>
+            <v>46059.648170324072</v>
           </cell>
           <cell r="L10">
-            <v>33.24</v>
+            <v>33.49</v>
           </cell>
         </row>
         <row r="11">
@@ -711,10 +710,10 @@
             <v>8.8187999999999995</v>
           </cell>
           <cell r="J11">
-            <v>46056.366570081016</v>
+            <v>46059.648170324072</v>
           </cell>
           <cell r="L11">
-            <v>9.2200000000000006</v>
+            <v>9.1660000000000004</v>
           </cell>
         </row>
         <row r="12">
@@ -734,10 +733,10 @@
             <v>42.381100000000004</v>
           </cell>
           <cell r="J12">
-            <v>46056.366570081016</v>
+            <v>46059.648170324072</v>
           </cell>
           <cell r="L12">
-            <v>37.895000000000003</v>
+            <v>38.619999999999997</v>
           </cell>
         </row>
         <row r="13">
@@ -757,10 +756,10 @@
             <v>79.260800000000003</v>
           </cell>
           <cell r="J13">
-            <v>46056.366570081016</v>
+            <v>46059.648170324072</v>
           </cell>
           <cell r="L13">
-            <v>153.02000000000001</v>
+            <v>154.54</v>
           </cell>
         </row>
         <row r="14">
@@ -780,10 +779,10 @@
             <v>188.8296</v>
           </cell>
           <cell r="J14">
-            <v>46056.366570081016</v>
+            <v>46059.648170324072</v>
           </cell>
           <cell r="L14">
-            <v>385.74</v>
+            <v>390.66</v>
           </cell>
         </row>
         <row r="15">
@@ -803,10 +802,10 @@
             <v>108.09699999999999</v>
           </cell>
           <cell r="J15">
-            <v>46056.366570081016</v>
+            <v>46059.648170324072</v>
           </cell>
           <cell r="L15">
-            <v>113.44</v>
+            <v>111.77</v>
           </cell>
         </row>
         <row r="16">
@@ -826,10 +825,10 @@
             <v>16.910799999999998</v>
           </cell>
           <cell r="J16">
-            <v>46056.366570081016</v>
+            <v>46059.648170324072</v>
           </cell>
           <cell r="L16">
-            <v>21.462599999999998</v>
+            <v>21.6112</v>
           </cell>
         </row>
         <row r="17">
@@ -849,10 +848,10 @@
             <v>183.25</v>
           </cell>
           <cell r="J17">
-            <v>46056.366570081016</v>
+            <v>46059.648170324072</v>
           </cell>
           <cell r="L17">
-            <v>180.55615999999998</v>
+            <v>175.20813000000001</v>
           </cell>
         </row>
         <row r="18">
@@ -872,10 +871,10 @@
             <v>86.142099999999999</v>
           </cell>
           <cell r="J18">
-            <v>46056.366570081016</v>
+            <v>46059.648170324072</v>
           </cell>
           <cell r="L18">
-            <v>136.03616</v>
+            <v>130.49978999999999</v>
           </cell>
         </row>
         <row r="19">
@@ -895,10 +894,10 @@
             <v>24.51</v>
           </cell>
           <cell r="J19">
-            <v>46056.366570081016</v>
+            <v>46059.648170324072</v>
           </cell>
           <cell r="L19">
-            <v>35.299799999999998</v>
+            <v>35.7044</v>
           </cell>
         </row>
         <row r="20">
@@ -918,10 +917,10 @@
             <v>188.49709999999999</v>
           </cell>
           <cell r="J20">
-            <v>46056.366570081016</v>
+            <v>46059.648170324072</v>
           </cell>
           <cell r="L20">
-            <v>210.91560000000001</v>
+            <v>211.02279999999999</v>
           </cell>
         </row>
         <row r="21">
@@ -941,10 +940,10 @@
             <v>17.7333</v>
           </cell>
           <cell r="J21">
-            <v>46056.366570081016</v>
+            <v>46059.648170324072</v>
           </cell>
           <cell r="L21">
-            <v>26.828800000000001</v>
+            <v>27.180900000000001</v>
           </cell>
         </row>
         <row r="22">
@@ -964,10 +963,10 @@
             <v>1009.4647</v>
           </cell>
           <cell r="J22">
-            <v>46056.366570081016</v>
+            <v>46059.648170324072</v>
           </cell>
           <cell r="L22">
-            <v>1011</v>
+            <v>1020</v>
           </cell>
         </row>
         <row r="23">
@@ -987,10 +986,10 @@
             <v>97.022000000000006</v>
           </cell>
           <cell r="J23">
-            <v>46056.366570081016</v>
+            <v>46059.648170324072</v>
           </cell>
           <cell r="L23">
-            <v>99.4</v>
+            <v>96.4</v>
           </cell>
         </row>
         <row r="24">
@@ -1010,10 +1009,10 @@
             <v>93.194999999999993</v>
           </cell>
           <cell r="J24">
-            <v>46056.366570081016</v>
+            <v>46059.648170324072</v>
           </cell>
           <cell r="L24">
-            <v>98.9</v>
+            <v>94.09</v>
           </cell>
         </row>
       </sheetData>
@@ -1340,11 +1339,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{840B4B52-5CB9-41B5-89C1-B1D0A0795C06}">
-  <dimension ref="A1:N19"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2:F19"/>
+      <selection pane="bottomLeft" activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1354,708 +1353,729 @@
     <col min="3" max="3" width="9.36328125" customWidth="1"/>
     <col min="4" max="4" width="7.36328125" customWidth="1"/>
     <col min="5" max="5" width="18.36328125" customWidth="1"/>
-    <col min="6" max="6" width="23.90625" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.54296875" customWidth="1"/>
-    <col min="8" max="8" width="22.26953125" customWidth="1"/>
-    <col min="9" max="9" width="21.90625" customWidth="1"/>
-    <col min="11" max="11" width="12.6328125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.90625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.1796875" customWidth="1"/>
+    <col min="6" max="6" width="23.90625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.90625" customWidth="1"/>
+    <col min="9" max="9" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.90625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" s="20">
-        <f ca="1">SUM(K2:K19)</f>
-        <v>2934843.3182326802</v>
-      </c>
-      <c r="L1" s="19" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A2" s="21" t="str">
+      <c r="I1" s="15">
+        <f ca="1">SUM(I2:I24)</f>
+        <v>2933642.1897175703</v>
+      </c>
+      <c r="J1" s="14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A2" s="16" t="str">
         <f>[1]Portafoglio!B7</f>
         <v>AMUNDI ELTIF PIR AP</v>
       </c>
-      <c r="B2" s="22" t="str">
+      <c r="B2" s="17" t="str">
         <f>[1]Portafoglio!C7</f>
         <v>LU2906336990</v>
       </c>
-      <c r="C2" s="23">
+      <c r="C2" s="18">
         <f>[1]Portafoglio!D7</f>
         <v>99.85</v>
       </c>
-      <c r="D2" s="24" t="str">
+      <c r="D2" s="19" t="str">
         <f>[1]Portafoglio!E7</f>
         <v>EUR</v>
       </c>
-      <c r="E2" s="25">
+      <c r="E2" s="20">
         <f>[1]Portafoglio!F7</f>
         <v>100</v>
       </c>
-      <c r="F2" s="17">
+      <c r="F2" s="13">
         <f>TRUNC([1]Portafoglio!J7)</f>
-        <v>46056</v>
-      </c>
-      <c r="G2" s="16"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="28">
+        <v>46059</v>
+      </c>
+      <c r="G2" s="23">
         <f ca="1">[1]Portafoglio!L7</f>
         <v>100.77</v>
       </c>
-      <c r="K2" s="26">
-        <f ca="1">+C2*I2</f>
+      <c r="I2" s="26">
+        <f ca="1">+C2*G2</f>
         <v>10061.884499999998</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A3" s="21" t="str">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A3" s="16" t="str">
         <f>[1]Portafoglio!B8</f>
         <v>BSKT/BNPI 28</v>
       </c>
-      <c r="B3" s="22" t="str">
+      <c r="B3" s="17" t="str">
         <f>[1]Portafoglio!C8</f>
         <v>XS3174997521</v>
       </c>
-      <c r="C3" s="23">
+      <c r="C3" s="18">
         <f>[1]Portafoglio!D8</f>
         <v>155</v>
       </c>
-      <c r="D3" s="24" t="str">
+      <c r="D3" s="19" t="str">
         <f>[1]Portafoglio!E8</f>
         <v>EUR</v>
       </c>
-      <c r="E3" s="25">
+      <c r="E3" s="20">
         <f>[1]Portafoglio!F8</f>
         <v>94.621300000000005</v>
       </c>
-      <c r="F3" s="17">
+      <c r="F3" s="13">
         <f>TRUNC([1]Portafoglio!J8)</f>
-        <v>46056</v>
-      </c>
-      <c r="G3" s="16"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="28">
+        <v>46059</v>
+      </c>
+      <c r="G3" s="23">
         <f ca="1">[1]Portafoglio!L8</f>
-        <v>95.99</v>
-      </c>
-      <c r="K3" s="26">
-        <f t="shared" ref="K3:K19" ca="1" si="0">+C3*I3</f>
-        <v>14878.449999999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A4" s="21" t="str">
+        <v>87.06</v>
+      </c>
+      <c r="I3" s="26">
+        <f ca="1">+C3*G3</f>
+        <v>13494.300000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A4" s="16" t="str">
         <f>[1]Portafoglio!B9</f>
         <v>BTP01.03.22-01.04.27</v>
       </c>
-      <c r="B4" s="22" t="str">
+      <c r="B4" s="17" t="str">
         <f>[1]Portafoglio!C9</f>
         <v>IT0005484552</v>
       </c>
-      <c r="C4" s="23">
+      <c r="C4" s="18">
         <f>[1]Portafoglio!D9</f>
         <v>25000</v>
       </c>
-      <c r="D4" s="24" t="str">
+      <c r="D4" s="19" t="str">
         <f>[1]Portafoglio!E9</f>
         <v>EUR</v>
       </c>
-      <c r="E4" s="25">
+      <c r="E4" s="20">
         <f>[1]Portafoglio!F9</f>
         <v>90.380700000000004</v>
       </c>
-      <c r="F4" s="17">
+      <c r="F4" s="13">
         <f>TRUNC([1]Portafoglio!J9)</f>
-        <v>46056</v>
-      </c>
-      <c r="G4" s="16"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="28">
+        <v>46059</v>
+      </c>
+      <c r="G4" s="23">
         <f ca="1">[1]Portafoglio!L9</f>
-        <v>98.96</v>
-      </c>
-      <c r="K4" s="26">
-        <f t="shared" ca="1" si="0"/>
-        <v>2474000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A5" s="21" t="str">
+        <v>98.94</v>
+      </c>
+      <c r="I4" s="26">
+        <f ca="1">+C4*G4</f>
+        <v>2473500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A5" s="16" t="str">
         <f>[1]Portafoglio!B10</f>
         <v>FID ASIA AGGR AC EUR</v>
       </c>
-      <c r="B5" s="22" t="str">
+      <c r="B5" s="17" t="str">
         <f>[1]Portafoglio!C10</f>
         <v>LU0345361124</v>
       </c>
-      <c r="C5" s="23">
+      <c r="C5" s="18">
         <f>[1]Portafoglio!D10</f>
         <v>786.29</v>
       </c>
-      <c r="D5" s="24" t="str">
+      <c r="D5" s="19" t="str">
         <f>[1]Portafoglio!E10</f>
         <v>EUR</v>
       </c>
-      <c r="E5" s="25">
+      <c r="E5" s="20">
         <f>[1]Portafoglio!F10</f>
         <v>31.14</v>
       </c>
-      <c r="F5" s="17">
+      <c r="F5" s="13">
         <f>TRUNC([1]Portafoglio!J10)</f>
-        <v>46056</v>
-      </c>
-      <c r="G5" s="16"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="28">
+        <v>46059</v>
+      </c>
+      <c r="G5" s="23">
         <f ca="1">[1]Portafoglio!L10</f>
-        <v>33.24</v>
-      </c>
-      <c r="K5" s="26">
-        <f t="shared" ca="1" si="0"/>
-        <v>26136.279600000002</v>
-      </c>
-      <c r="M5" s="26"/>
-      <c r="N5" s="27"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A6" s="21" t="str">
+        <v>33.49</v>
+      </c>
+      <c r="I5" s="26">
+        <f ca="1">+C5*G5</f>
+        <v>26332.8521</v>
+      </c>
+      <c r="K5" s="21"/>
+      <c r="L5" s="22"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A6" s="16" t="str">
         <f>[1]Portafoglio!B11</f>
         <v>FID GLO QLTY USD EUR</v>
       </c>
-      <c r="B6" s="22" t="str">
+      <c r="B6" s="17" t="str">
         <f>[1]Portafoglio!C11</f>
         <v>IE00BYXVGZ48</v>
       </c>
-      <c r="C6" s="23">
+      <c r="C6" s="18">
         <f>[1]Portafoglio!D11</f>
         <v>570</v>
       </c>
-      <c r="D6" s="24" t="str">
+      <c r="D6" s="19" t="str">
         <f>[1]Portafoglio!E11</f>
         <v>EUR</v>
       </c>
-      <c r="E6" s="25">
+      <c r="E6" s="20">
         <f>[1]Portafoglio!F11</f>
         <v>8.8187999999999995</v>
       </c>
-      <c r="F6" s="17">
+      <c r="F6" s="13">
         <f>TRUNC([1]Portafoglio!J11)</f>
-        <v>46056</v>
-      </c>
-      <c r="G6" s="16"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="28">
+        <v>46059</v>
+      </c>
+      <c r="G6" s="23">
         <f ca="1">[1]Portafoglio!L11</f>
-        <v>9.2200000000000006</v>
-      </c>
-      <c r="K6" s="26">
-        <f t="shared" ca="1" si="0"/>
-        <v>5255.4000000000005</v>
-      </c>
-      <c r="M6" s="26"/>
-      <c r="N6" s="27"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A7" s="21" t="str">
+        <v>9.1660000000000004</v>
+      </c>
+      <c r="I6" s="26">
+        <f ca="1">+C6*G6</f>
+        <v>5224.62</v>
+      </c>
+      <c r="K6" s="21"/>
+      <c r="L6" s="22"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A7" s="16" t="str">
         <f>[1]Portafoglio!B12</f>
         <v>GLB X SILV USD-A EUR</v>
       </c>
-      <c r="B7" s="22" t="str">
+      <c r="B7" s="17" t="str">
         <f>[1]Portafoglio!C12</f>
         <v>IE000UL6CLP7</v>
       </c>
-      <c r="C7" s="23">
+      <c r="C7" s="18">
         <f>[1]Portafoglio!D12</f>
         <v>237</v>
       </c>
-      <c r="D7" s="24" t="str">
+      <c r="D7" s="19" t="str">
         <f>[1]Portafoglio!E12</f>
         <v>EUR</v>
       </c>
-      <c r="E7" s="25">
+      <c r="E7" s="20">
         <f>[1]Portafoglio!F12</f>
         <v>42.381100000000004</v>
       </c>
-      <c r="F7" s="17">
+      <c r="F7" s="13">
         <f>TRUNC([1]Portafoglio!J12)</f>
-        <v>46056</v>
-      </c>
-      <c r="G7" s="16"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="28">
+        <v>46059</v>
+      </c>
+      <c r="G7" s="23">
         <f ca="1">[1]Portafoglio!L12</f>
-        <v>37.895000000000003</v>
-      </c>
-      <c r="K7" s="26">
-        <f t="shared" ca="1" si="0"/>
-        <v>8981.1150000000016</v>
-      </c>
-      <c r="M7" s="26"/>
-      <c r="N7" s="27"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A8" s="21" t="str">
+        <v>38.619999999999997</v>
+      </c>
+      <c r="I7" s="26">
+        <f ca="1">+C7*G7</f>
+        <v>9152.9399999999987</v>
+      </c>
+      <c r="K7" s="21"/>
+      <c r="L7" s="22"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A8" s="16" t="str">
         <f>[1]Portafoglio!B13</f>
         <v>H2O MULTIBONDS R EUR</v>
       </c>
-      <c r="B8" s="22" t="str">
+      <c r="B8" s="17" t="str">
         <f>[1]Portafoglio!C13</f>
         <v>FR0013393329</v>
       </c>
-      <c r="C8" s="23">
+      <c r="C8" s="18">
         <f>[1]Portafoglio!D13</f>
         <v>808.88599999999997</v>
       </c>
-      <c r="D8" s="24" t="str">
+      <c r="D8" s="19" t="str">
         <f>[1]Portafoglio!E13</f>
         <v>EUR</v>
       </c>
-      <c r="E8" s="25">
+      <c r="E8" s="20">
         <f>[1]Portafoglio!F13</f>
         <v>79.260800000000003</v>
       </c>
-      <c r="F8" s="17">
+      <c r="F8" s="13">
         <f>TRUNC([1]Portafoglio!J13)</f>
-        <v>46056</v>
-      </c>
-      <c r="G8" s="16"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="28">
+        <v>46059</v>
+      </c>
+      <c r="G8" s="23">
         <f ca="1">[1]Portafoglio!L13</f>
-        <v>153.02000000000001</v>
-      </c>
-      <c r="K8" s="26">
-        <f t="shared" ca="1" si="0"/>
-        <v>123775.73572</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A9" s="21" t="str">
+        <v>154.54</v>
+      </c>
+      <c r="I8" s="26">
+        <f ca="1">+C8*G8</f>
+        <v>125005.24243999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A9" s="16" t="str">
         <f>[1]Portafoglio!B14</f>
         <v>H2O MULTISTRATEGIES</v>
       </c>
-      <c r="B9" s="22" t="str">
+      <c r="B9" s="17" t="str">
         <f>[1]Portafoglio!C14</f>
         <v>FR0010923383</v>
       </c>
-      <c r="C9" s="23">
+      <c r="C9" s="18">
         <f>[1]Portafoglio!D14</f>
         <v>255.42699999999999</v>
       </c>
-      <c r="D9" s="24" t="str">
+      <c r="D9" s="19" t="str">
         <f>[1]Portafoglio!E14</f>
         <v>EUR</v>
       </c>
-      <c r="E9" s="25">
+      <c r="E9" s="20">
         <f>[1]Portafoglio!F14</f>
         <v>188.8296</v>
       </c>
-      <c r="F9" s="17">
+      <c r="F9" s="13">
         <f>TRUNC([1]Portafoglio!J14)</f>
-        <v>46056</v>
-      </c>
-      <c r="G9" s="16"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="28">
+        <v>46059</v>
+      </c>
+      <c r="G9" s="23">
         <f ca="1">[1]Portafoglio!L14</f>
-        <v>385.74</v>
-      </c>
-      <c r="K9" s="26">
-        <f t="shared" ca="1" si="0"/>
-        <v>98528.410980000001</v>
-      </c>
-      <c r="M9" s="26"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A10" s="21" t="str">
+        <v>390.66</v>
+      </c>
+      <c r="I9" s="26">
+        <f ca="1">+C9*G9</f>
+        <v>99785.111820000006</v>
+      </c>
+      <c r="K9" s="21"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A10" s="16" t="str">
         <f>[1]Portafoglio!B15</f>
         <v>ISHS MSCI WORLD EUR</v>
       </c>
-      <c r="B10" s="22" t="str">
+      <c r="B10" s="17" t="str">
         <f>[1]Portafoglio!C15</f>
         <v>IE00B4L5Y983</v>
       </c>
-      <c r="C10" s="23">
+      <c r="C10" s="18">
         <f>[1]Portafoglio!D15</f>
         <v>47</v>
       </c>
-      <c r="D10" s="24" t="str">
+      <c r="D10" s="19" t="str">
         <f>[1]Portafoglio!E15</f>
         <v>EUR</v>
       </c>
-      <c r="E10" s="25">
+      <c r="E10" s="20">
         <f>[1]Portafoglio!F15</f>
         <v>108.09699999999999</v>
       </c>
-      <c r="F10" s="17">
+      <c r="F10" s="13">
         <f>TRUNC([1]Portafoglio!J15)</f>
-        <v>46056</v>
-      </c>
-      <c r="G10" s="16"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="28">
+        <v>46059</v>
+      </c>
+      <c r="G10" s="23">
         <f ca="1">[1]Portafoglio!L15</f>
-        <v>113.44</v>
-      </c>
-      <c r="K10" s="26">
-        <f t="shared" ca="1" si="0"/>
-        <v>5331.68</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A11" s="21" t="str">
+        <v>111.77</v>
+      </c>
+      <c r="I10" s="26">
+        <f ca="1">+C10*G10</f>
+        <v>5253.19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A11" s="16" t="str">
         <f>[1]Portafoglio!B16</f>
         <v>M&amp;G EUROP STRA VAL A</v>
       </c>
-      <c r="B11" s="22" t="str">
+      <c r="B11" s="17" t="str">
         <f>[1]Portafoglio!C16</f>
         <v>LU1670707527</v>
       </c>
-      <c r="C11" s="23">
+      <c r="C11" s="18">
         <f>[1]Portafoglio!D16</f>
         <v>945.54899999999998</v>
       </c>
-      <c r="D11" s="24" t="str">
+      <c r="D11" s="19" t="str">
         <f>[1]Portafoglio!E16</f>
         <v>EUR</v>
       </c>
-      <c r="E11" s="25">
+      <c r="E11" s="20">
         <f>[1]Portafoglio!F16</f>
         <v>16.910799999999998</v>
       </c>
-      <c r="F11" s="17">
+      <c r="F11" s="13">
         <f>TRUNC([1]Portafoglio!J16)</f>
-        <v>46056</v>
-      </c>
-      <c r="G11" s="16"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="28">
+        <v>46059</v>
+      </c>
+      <c r="G11" s="23">
         <f ca="1">[1]Portafoglio!L16</f>
-        <v>21.462599999999998</v>
-      </c>
-      <c r="K11" s="26">
-        <f t="shared" ca="1" si="0"/>
-        <v>20293.939967399998</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A12" s="21" t="str">
+        <v>21.6112</v>
+      </c>
+      <c r="I11" s="26">
+        <f ca="1">+C11*G11</f>
+        <v>20434.448548799999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A12" s="16" t="str">
         <f>[1]Portafoglio!B17</f>
         <v>MSIF GL BRDS AC</v>
       </c>
-      <c r="B12" s="22" t="str">
+      <c r="B12" s="17" t="str">
         <f>[1]Portafoglio!C17</f>
         <v>LU0119620416</v>
       </c>
-      <c r="C12" s="23">
+      <c r="C12" s="18">
         <f>[1]Portafoglio!D17</f>
         <v>104.37</v>
       </c>
-      <c r="D12" s="24" t="str">
+      <c r="D12" s="19" t="str">
         <f>[1]Portafoglio!E17</f>
         <v>USD</v>
       </c>
-      <c r="E12" s="25">
+      <c r="E12" s="20">
         <f>[1]Portafoglio!F17</f>
         <v>183.25</v>
       </c>
-      <c r="F12" s="17">
+      <c r="F12" s="13">
         <f>TRUNC([1]Portafoglio!J17)</f>
-        <v>46056</v>
-      </c>
-      <c r="G12" s="16"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="28">
+        <v>46059</v>
+      </c>
+      <c r="G12" s="23">
         <f ca="1">[1]Portafoglio!L17</f>
-        <v>180.55615999999998</v>
-      </c>
-      <c r="K12" s="26">
-        <f t="shared" ca="1" si="0"/>
-        <v>18844.646419199998</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A13" s="21" t="str">
+        <v>175.20813000000001</v>
+      </c>
+      <c r="I12" s="26">
+        <f ca="1">+C12*G12</f>
+        <v>18286.472528100003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A13" s="16" t="str">
         <f>[1]Portafoglio!B18</f>
         <v>MSIF GL OPP AC</v>
       </c>
-      <c r="B13" s="22" t="str">
+      <c r="B13" s="17" t="str">
         <f>[1]Portafoglio!C18</f>
         <v>LU0552385295</v>
       </c>
-      <c r="C13" s="23">
+      <c r="C13" s="18">
         <f>[1]Portafoglio!D18</f>
         <v>207.953</v>
       </c>
-      <c r="D13" s="24" t="str">
+      <c r="D13" s="19" t="str">
         <f>[1]Portafoglio!E18</f>
         <v>USD</v>
       </c>
-      <c r="E13" s="25">
+      <c r="E13" s="20">
         <f>[1]Portafoglio!F18</f>
         <v>86.142099999999999</v>
       </c>
-      <c r="F13" s="17">
+      <c r="F13" s="13">
         <f>TRUNC([1]Portafoglio!J18)</f>
-        <v>46056</v>
-      </c>
-      <c r="G13" s="16"/>
-      <c r="H13" s="18"/>
-      <c r="I13" s="28">
+        <v>46059</v>
+      </c>
+      <c r="G13" s="23">
         <f ca="1">[1]Portafoglio!L18</f>
-        <v>136.03616</v>
-      </c>
-      <c r="K13" s="26">
-        <f t="shared" ca="1" si="0"/>
-        <v>28289.127580479999</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A14" s="21" t="str">
+        <v>130.49978999999999</v>
+      </c>
+      <c r="I13" s="26">
+        <f ca="1">+C13*G13</f>
+        <v>27137.822829869998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A14" s="16" t="str">
         <f>[1]Portafoglio!B19</f>
         <v>N1 CLIM ENV EQ B EUR</v>
       </c>
-      <c r="B14" s="22" t="str">
+      <c r="B14" s="17" t="str">
         <f>[1]Portafoglio!C19</f>
         <v>LU0348926287</v>
       </c>
-      <c r="C14" s="23">
+      <c r="C14" s="18">
         <f>[1]Portafoglio!D19</f>
         <v>448.18400000000003</v>
       </c>
-      <c r="D14" s="24" t="str">
+      <c r="D14" s="19" t="str">
         <f>[1]Portafoglio!E19</f>
         <v>EUR</v>
       </c>
-      <c r="E14" s="25">
+      <c r="E14" s="20">
         <f>[1]Portafoglio!F19</f>
         <v>24.51</v>
       </c>
-      <c r="F14" s="17">
+      <c r="F14" s="13">
         <f>TRUNC([1]Portafoglio!J19)</f>
-        <v>46056</v>
-      </c>
-      <c r="G14" s="16"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="28">
+        <v>46059</v>
+      </c>
+      <c r="G14" s="23">
         <f ca="1">[1]Portafoglio!L19</f>
-        <v>35.299799999999998</v>
-      </c>
-      <c r="K14" s="26">
-        <f t="shared" ca="1" si="0"/>
-        <v>15820.8055632</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A15" s="21" t="str">
+        <v>35.7044</v>
+      </c>
+      <c r="I14" s="26">
+        <f ca="1">+C14*G14</f>
+        <v>16002.140809600001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A15" s="16" t="str">
         <f>[1]Portafoglio!B20</f>
         <v>N1 EUR BANK D BP EUR</v>
       </c>
-      <c r="B15" s="22" t="str">
+      <c r="B15" s="17" t="str">
         <f>[1]Portafoglio!C20</f>
         <v>LU0772944145</v>
       </c>
-      <c r="C15" s="23">
+      <c r="C15" s="18">
         <f>[1]Portafoglio!D20</f>
         <v>117.944</v>
       </c>
-      <c r="D15" s="24" t="str">
+      <c r="D15" s="19" t="str">
         <f>[1]Portafoglio!E20</f>
         <v>EUR</v>
       </c>
-      <c r="E15" s="25">
+      <c r="E15" s="20">
         <f>[1]Portafoglio!F20</f>
         <v>188.49709999999999</v>
       </c>
-      <c r="F15" s="17">
+      <c r="F15" s="13">
         <f>TRUNC([1]Portafoglio!J20)</f>
-        <v>46056</v>
-      </c>
-      <c r="G15" s="16"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="28">
+        <v>46059</v>
+      </c>
+      <c r="G15" s="23">
         <f ca="1">[1]Portafoglio!L20</f>
-        <v>210.91560000000001</v>
-      </c>
-      <c r="K15" s="26">
-        <f t="shared" ca="1" si="0"/>
-        <v>24876.229526400002</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A16" s="21" t="str">
+        <v>211.02279999999999</v>
+      </c>
+      <c r="I15" s="26">
+        <f ca="1">+C15*G15</f>
+        <v>24888.873123199999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A16" s="16" t="str">
         <f>[1]Portafoglio!B21</f>
         <v>SISF ASIAN OP AC EUR</v>
       </c>
-      <c r="B16" s="22" t="str">
+      <c r="B16" s="17" t="str">
         <f>[1]Portafoglio!C21</f>
         <v>LU0248184466</v>
       </c>
-      <c r="C16" s="23">
+      <c r="C16" s="18">
         <f>[1]Portafoglio!D21</f>
         <v>586.02</v>
       </c>
-      <c r="D16" s="24" t="str">
+      <c r="D16" s="19" t="str">
         <f>[1]Portafoglio!E21</f>
         <v>EUR</v>
       </c>
-      <c r="E16" s="25">
+      <c r="E16" s="20">
         <f>[1]Portafoglio!F21</f>
         <v>17.7333</v>
       </c>
-      <c r="F16" s="17">
+      <c r="F16" s="13">
         <f>TRUNC([1]Portafoglio!J21)</f>
-        <v>46056</v>
-      </c>
-      <c r="G16" s="16"/>
-      <c r="H16" s="18"/>
-      <c r="I16" s="28">
+        <v>46059</v>
+      </c>
+      <c r="G16" s="23">
         <f ca="1">[1]Portafoglio!L21</f>
-        <v>26.828800000000001</v>
-      </c>
-      <c r="K16" s="26">
-        <f t="shared" ca="1" si="0"/>
-        <v>15722.213376</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A17" s="21" t="str">
+        <v>27.180900000000001</v>
+      </c>
+      <c r="I16" s="26">
+        <f ca="1">+C16*G16</f>
+        <v>15928.551018</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A17" s="16" t="str">
         <f>[1]Portafoglio!B22</f>
         <v>VON EXPE28</v>
       </c>
-      <c r="B17" s="22" t="str">
+      <c r="B17" s="17" t="str">
         <f>[1]Portafoglio!C22</f>
         <v>DE000VJ0K5X0</v>
       </c>
-      <c r="C17" s="23">
+      <c r="C17" s="18">
         <f>[1]Portafoglio!D22</f>
         <v>15</v>
       </c>
-      <c r="D17" s="24" t="str">
+      <c r="D17" s="19" t="str">
         <f>[1]Portafoglio!E22</f>
         <v>EUR</v>
       </c>
-      <c r="E17" s="25">
+      <c r="E17" s="20">
         <f>[1]Portafoglio!F22</f>
         <v>1009.4647</v>
       </c>
-      <c r="F17" s="17">
+      <c r="F17" s="13">
         <f>TRUNC([1]Portafoglio!J22)</f>
-        <v>46056</v>
-      </c>
-      <c r="G17" s="16"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="28">
+        <v>46059</v>
+      </c>
+      <c r="G17" s="23">
         <f ca="1">[1]Portafoglio!L22</f>
-        <v>1011</v>
-      </c>
-      <c r="K17" s="26">
-        <f t="shared" ca="1" si="0"/>
-        <v>15165</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A18" s="21" t="str">
+        <v>1020</v>
+      </c>
+      <c r="I17" s="26">
+        <f ca="1">+C17*G17</f>
+        <v>15300</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A18" s="16" t="str">
         <f>[1]Portafoglio!B23</f>
         <v>VON EXPE29</v>
       </c>
-      <c r="B18" s="22" t="str">
+      <c r="B18" s="17" t="str">
         <f>[1]Portafoglio!C23</f>
         <v>DE000VJ20861</v>
       </c>
-      <c r="C18" s="23">
+      <c r="C18" s="18">
         <f>[1]Portafoglio!D23</f>
         <v>205</v>
       </c>
-      <c r="D18" s="24" t="str">
+      <c r="D18" s="19" t="str">
         <f>[1]Portafoglio!E23</f>
         <v>EUR</v>
       </c>
-      <c r="E18" s="25">
+      <c r="E18" s="20">
         <f>[1]Portafoglio!F23</f>
         <v>97.022000000000006</v>
       </c>
-      <c r="F18" s="17">
+      <c r="F18" s="13">
         <f>TRUNC([1]Portafoglio!J23)</f>
-        <v>46056</v>
-      </c>
-      <c r="G18" s="16"/>
-      <c r="H18" s="18"/>
-      <c r="I18" s="28">
+        <v>46059</v>
+      </c>
+      <c r="G18" s="23">
         <f ca="1">[1]Portafoglio!L23</f>
-        <v>99.4</v>
-      </c>
-      <c r="K18" s="26">
-        <f t="shared" ca="1" si="0"/>
-        <v>20377</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A19" s="21" t="str">
+        <v>96.4</v>
+      </c>
+      <c r="I18" s="26">
+        <f ca="1">+C18*G18</f>
+        <v>19762</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A19" s="16" t="str">
         <f>[1]Portafoglio!B24</f>
         <v>XTRACKERS INFORM EUR</v>
       </c>
-      <c r="B19" s="22" t="str">
+      <c r="B19" s="17" t="str">
         <f>[1]Portafoglio!C24</f>
         <v>IE00BM67HT60</v>
       </c>
-      <c r="C19" s="23">
+      <c r="C19" s="18">
         <f>[1]Portafoglio!D24</f>
         <v>86</v>
       </c>
-      <c r="D19" s="24" t="str">
+      <c r="D19" s="19" t="str">
         <f>[1]Portafoglio!E24</f>
         <v>EUR</v>
       </c>
-      <c r="E19" s="25">
+      <c r="E19" s="20">
         <f>[1]Portafoglio!F24</f>
         <v>93.194999999999993</v>
       </c>
-      <c r="F19" s="17">
+      <c r="F19" s="13">
         <f>TRUNC([1]Portafoglio!J24)</f>
-        <v>46056</v>
-      </c>
-      <c r="G19" s="16"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="28">
+        <v>46059</v>
+      </c>
+      <c r="G19" s="23">
         <f ca="1">[1]Portafoglio!L24</f>
-        <v>98.9</v>
-      </c>
-      <c r="K19" s="26">
-        <f t="shared" ca="1" si="0"/>
-        <v>8505.4</v>
+        <v>94.09</v>
+      </c>
+      <c r="I19" s="26">
+        <f ca="1">+C19*G19</f>
+        <v>8091.7400000000007</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A20" s="16"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="23"/>
+      <c r="I20" s="26">
+        <f t="shared" ref="I20:I24" si="0">+C20*G20</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A21" s="16"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="23"/>
+      <c r="I21" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A22" s="16"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="23"/>
+      <c r="I22" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A23" s="16"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="23"/>
+      <c r="I23" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A24" s="16"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="23"/>
+      <c r="I24" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:A19">
+  <conditionalFormatting sqref="A2:A24">
     <cfRule type="expression" dxfId="5" priority="3" stopIfTrue="1">
       <formula>IF(AND(ISNUMBER(SEARCH("H2O", A2)), ISNUMBER(SEARCH("SP", A2))), 1,0)</formula>
     </cfRule>
@@ -2063,7 +2083,7 @@
       <formula>NOT(ISERROR(SEARCH("BTP",A2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D19">
+  <conditionalFormatting sqref="D2:D24">
     <cfRule type="notContainsText" dxfId="2" priority="2" operator="notContains" text="EUR">
       <formula>ISERROR(SEARCH("EUR",D2))</formula>
     </cfRule>
@@ -2085,7 +2105,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>D2:D19</xm:sqref>
+          <xm:sqref>D2:D24</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -2109,255 +2129,255 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="9">
+        <v>45002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="2">
+        <v>45002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="9">
+        <v>45355</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="8" t="s">
+      <c r="C5" s="2">
+        <v>45355</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B6" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="12">
-        <v>45002</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
+      <c r="C6" s="9">
+        <v>45355</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="2">
+        <v>45355</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="9">
+        <v>45355</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="2">
+        <v>45355</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="2">
+        <v>45355</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="9">
+        <v>45355</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="2">
+        <v>45355</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="9">
+        <v>45701</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B14" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="5">
-        <v>45002</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="12">
-        <v>45355</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="4" t="s">
+      <c r="C14" s="2">
+        <v>45702</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="2">
+        <v>45702</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="9">
+        <v>45702</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B17" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="5">
-        <v>45355</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6" s="12">
-        <v>45355</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="4" t="s">
+      <c r="C17" s="9">
+        <v>45705</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="2">
+        <v>45706</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B19" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="5">
-        <v>45355</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="C8" s="12">
-        <v>45355</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C9" s="5">
-        <v>45355</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C10" s="5">
-        <v>45355</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="C11" s="12">
-        <v>45355</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" s="4" t="s">
+      <c r="C19" s="9">
+        <v>45806</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" s="10">
+        <v>46044</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="11">
+        <v>46044</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" s="2">
+        <v>46044</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B23" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C12" s="5">
-        <v>45355</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="C13" s="12">
-        <v>45701</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" s="5">
-        <v>45702</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C15" s="5">
-        <v>45702</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C16" s="12">
-        <v>45702</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C17" s="12">
-        <v>45705</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C18" s="5">
-        <v>45706</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="C19" s="12">
-        <v>45806</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="C20" s="13">
-        <v>46044</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="C21" s="14">
-        <v>46044</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A22" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C22" s="5">
-        <v>46044</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A23" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B23" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="C23" s="13">
+      <c r="C23" s="10">
         <v>46048</v>
       </c>
     </row>

</xml_diff>